<commit_message>
fix(week): fix week 14
</commit_message>
<xml_diff>
--- a/content/_data/NFL 2023 week 14.xlsx
+++ b/content/_data/NFL 2023 week 14.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Football 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendavidson/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6790733A-EFD3-40D5-A6B8-7B45640D4009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24307A88-C980-9841-AA49-80491839ECB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>** WEEK # 14**</t>
   </si>
   <si>
-    <t>PITT  -5 1/2  pitt</t>
-  </si>
-  <si>
     <t>ATL  -1 1/2  t.b.</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>S.F.**</t>
+  </si>
+  <si>
+    <t>PITT  -5 1/2  N.E.</t>
   </si>
 </sst>
 </file>
@@ -1198,21 +1198,21 @@
   <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="74" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="10" width="13.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="0.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="10" width="13.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="0.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="31.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="31" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D1" s="7" t="s">
         <v>35</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="M1" s="8"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:21" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
@@ -1265,236 +1265,236 @@
       <c r="N2" s="11"/>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J3" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="32"/>
       <c r="M3" s="34" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="N3" s="33"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="32"/>
       <c r="M4" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N4" s="33"/>
       <c r="O4" s="45"/>
     </row>
-    <row r="5" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K5" s="12"/>
       <c r="L5" s="32"/>
       <c r="M5" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5" s="33"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H6" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="32"/>
       <c r="M6" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N6" s="33"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G7" s="50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="32"/>
       <c r="M7" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N7" s="55"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H8" s="51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I8" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="32"/>
       <c r="M8" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N8" s="33"/>
       <c r="O8" s="4"/>
@@ -1502,85 +1502,85 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="32"/>
       <c r="M9" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9" s="55"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I10" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J10" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="32"/>
       <c r="M10" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N10" s="33"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51"/>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -1597,163 +1597,163 @@
       <c r="N11" s="55"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H12" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I12" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J12" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="32"/>
       <c r="M12" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N12" s="33"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G13" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H13" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J13" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="32"/>
       <c r="M13" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N13" s="55"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="32"/>
       <c r="M14" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N14" s="33"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G15" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I15" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J15" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="32"/>
       <c r="M15" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N15" s="33"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50"/>
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
@@ -1770,46 +1770,46 @@
       <c r="N16" s="33"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H17" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I17" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J17" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="32"/>
       <c r="M17" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N17" s="33"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50"/>
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
@@ -1826,85 +1826,85 @@
       <c r="N18" s="33"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="32"/>
       <c r="M19" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N19" s="33"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I20" s="66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J20" s="66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K20" s="12"/>
       <c r="L20" s="32"/>
       <c r="M20" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N20" s="55"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="54"/>
       <c r="B21" s="54"/>
       <c r="C21" s="50"/>
@@ -1921,7 +1921,7 @@
       <c r="N21" s="33"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="60">
         <v>42</v>
       </c>
@@ -1958,7 +1958,7 @@
       <c r="N22" s="33"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="54"/>
       <c r="B23" s="54"/>
       <c r="C23" s="54"/>
@@ -1975,7 +1975,7 @@
       <c r="N23" s="55"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="60"/>
       <c r="B24" s="60"/>
       <c r="C24" s="65"/>
@@ -1992,7 +1992,7 @@
       <c r="N24" s="33"/>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="52"/>
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
@@ -2011,7 +2011,7 @@
       </c>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="16"/>
@@ -2028,7 +2028,7 @@
       <c r="N26" s="17"/>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:15" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>7</v>
       </c>
@@ -2069,36 +2069,36 @@
       </c>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G28" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H28" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I28" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J28" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="47">
@@ -2112,36 +2112,36 @@
       </c>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G29" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H29" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I29" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J29" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K29" s="12"/>
       <c r="L29" s="20">
@@ -2155,36 +2155,36 @@
       </c>
       <c r="O29" s="4"/>
     </row>
-    <row r="30" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G30" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H30" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J30" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K30" s="21"/>
       <c r="L30" s="20">
@@ -2198,36 +2198,36 @@
       </c>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G31" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J31" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="20">
@@ -2241,36 +2241,36 @@
       </c>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I32" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J32" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K32" s="12"/>
       <c r="L32" s="20">
@@ -2284,36 +2284,36 @@
       </c>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J33" s="51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="22">
@@ -2327,36 +2327,36 @@
       </c>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E34" s="50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F34" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G34" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H34" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I34" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J34" s="50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K34" s="12"/>
       <c r="L34" s="20">
@@ -2370,36 +2370,36 @@
       </c>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D35" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E35" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F35" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G35" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H35" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I35" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J35" s="50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K35" s="12"/>
       <c r="L35" s="22">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="51"/>
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
@@ -2436,36 +2436,36 @@
       </c>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E37" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F37" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G37" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H37" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I37" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J37" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K37" s="12"/>
       <c r="L37" s="22">
@@ -2479,36 +2479,36 @@
       </c>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F38" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H38" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I38" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J38" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="20">
@@ -2522,36 +2522,36 @@
       </c>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D39" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E39" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F39" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G39" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H39" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I39" s="50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J39" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K39" s="12"/>
       <c r="L39" s="22">
@@ -2565,36 +2565,36 @@
       </c>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G40" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H40" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I40" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J40" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K40" s="12"/>
       <c r="L40" s="20">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
       <c r="B41" s="50"/>
       <c r="C41" s="50"/>
@@ -2631,36 +2631,36 @@
       </c>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D42" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E42" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F42" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G42" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H42" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I42" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J42" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K42" s="12"/>
       <c r="L42" s="20">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="50"/>
       <c r="B43" s="50"/>
       <c r="C43" s="50"/>
@@ -2697,36 +2697,36 @@
       </c>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D44" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F44" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G44" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H44" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I44" s="51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J44" s="50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K44" s="12"/>
       <c r="L44" s="20">
@@ -2740,36 +2740,36 @@
       </c>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D45" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E45" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F45" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G45" s="66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H45" s="50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I45" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J45" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K45" s="23"/>
       <c r="L45" s="22">
@@ -2783,7 +2783,7 @@
       </c>
       <c r="O45" s="4"/>
     </row>
-    <row r="46" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="54"/>
       <c r="B46" s="51"/>
       <c r="C46" s="54"/>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="O46" s="4"/>
     </row>
-    <row r="47" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="57">
         <v>48.5</v>
       </c>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="O47" s="4"/>
     </row>
-    <row r="48" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="54"/>
       <c r="B48" s="50"/>
       <c r="C48" s="54"/>
@@ -2866,7 +2866,7 @@
       <c r="N48" s="56"/>
       <c r="O48" s="4"/>
     </row>
-    <row r="49" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="57"/>
       <c r="B49" s="57"/>
       <c r="C49" s="62"/>
@@ -2883,7 +2883,7 @@
       <c r="N49" s="19"/>
       <c r="O49" s="4"/>
     </row>
-    <row r="50" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="52"/>
       <c r="B50" s="52"/>
       <c r="C50" s="52"/>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="O50" s="4"/>
     </row>
-    <row r="51" spans="1:15" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2918,7 +2918,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
     </row>
-    <row r="52" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -2955,7 +2955,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2970,7 +2970,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>